<commit_message>
Added function to display meaning in error message.
</commit_message>
<xml_diff>
--- a/data/artikel.xlsx
+++ b/data/artikel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwt/Documents/Code/gelato/artikel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwt/Documents/Code/gelato/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1498AE-E8B5-8942-8570-9F73D55C9924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4992097F-9C8F-DD40-943C-D98D9866063E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="2020" windowWidth="28800" windowHeight="18000" xr2:uid="{2D6BCF81-A2D9-5B4D-AD53-B365A8194329}"/>
+    <workbookView xWindow="-36360" yWindow="-240" windowWidth="28800" windowHeight="18000" xr2:uid="{2D6BCF81-A2D9-5B4D-AD53-B365A8194329}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -591,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AD30F3-BC96-AA4E-AB81-F5562BDF30AC}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,15 +616,29 @@
         <v>63</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>64</v>
@@ -635,10 +649,10 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>64</v>
@@ -646,13 +660,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
         <v>64</v>
@@ -660,13 +674,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>64</v>
@@ -677,10 +691,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>64</v>
@@ -688,13 +702,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>64</v>
@@ -702,13 +716,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -716,13 +730,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
         <v>64</v>
@@ -730,55 +744,55 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
         <v>67</v>
@@ -789,10 +803,10 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
         <v>67</v>
@@ -800,13 +814,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>67</v>
@@ -814,13 +828,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
         <v>67</v>
@@ -831,10 +845,10 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
         <v>67</v>
@@ -842,13 +856,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
         <v>67</v>
@@ -856,13 +870,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
         <v>67</v>
@@ -870,13 +884,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
         <v>67</v>
@@ -887,10 +901,10 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
         <v>67</v>
@@ -898,13 +912,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
         <v>67</v>
@@ -912,13 +926,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
         <v>67</v>
@@ -926,13 +940,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
         <v>67</v>
@@ -940,13 +954,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
         <v>67</v>
@@ -954,13 +968,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
         <v>67</v>
@@ -971,10 +985,10 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
         <v>67</v>
@@ -982,29 +996,15 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added padding in analysis.
</commit_message>
<xml_diff>
--- a/data/artikel.xlsx
+++ b/data/artikel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwt/Documents/Code/gelato/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4992097F-9C8F-DD40-943C-D98D9866063E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E1343C-B129-864D-82A4-AADD5C7CD206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36360" yWindow="-240" windowWidth="28800" windowHeight="18000" xr2:uid="{2D6BCF81-A2D9-5B4D-AD53-B365A8194329}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2D6BCF81-A2D9-5B4D-AD53-B365A8194329}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="113">
   <si>
     <t>Artikel</t>
   </si>
@@ -240,6 +240,141 @@
   </si>
   <si>
     <t>Face</t>
+  </si>
+  <si>
+    <t>Gewürze</t>
+  </si>
+  <si>
+    <t>Gesicht</t>
+  </si>
+  <si>
+    <t>Sternanis</t>
+  </si>
+  <si>
+    <t>Lorbeerblatt</t>
+  </si>
+  <si>
+    <t>Koriander</t>
+  </si>
+  <si>
+    <t>Zimtrinde</t>
+  </si>
+  <si>
+    <t>Kurkuma</t>
+  </si>
+  <si>
+    <t>Currypulver</t>
+  </si>
+  <si>
+    <t>Paprika</t>
+  </si>
+  <si>
+    <t>Pfeffer</t>
+  </si>
+  <si>
+    <t>Muskatnuss</t>
+  </si>
+  <si>
+    <t>Kardamom</t>
+  </si>
+  <si>
+    <t>Nelken</t>
+  </si>
+  <si>
+    <t>Ingwer</t>
+  </si>
+  <si>
+    <t>Chiliflocken</t>
+  </si>
+  <si>
+    <t>Chilischote</t>
+  </si>
+  <si>
+    <t>Fenchel</t>
+  </si>
+  <si>
+    <t>Würzmittel und Soßen</t>
+  </si>
+  <si>
+    <t>Salz</t>
+  </si>
+  <si>
+    <t>Essig</t>
+  </si>
+  <si>
+    <t>Olivenöl</t>
+  </si>
+  <si>
+    <t>Salsa</t>
+  </si>
+  <si>
+    <t>Ketchup</t>
+  </si>
+  <si>
+    <t>Senf</t>
+  </si>
+  <si>
+    <t>Mayonnaise</t>
+  </si>
+  <si>
+    <t>Sojasoße</t>
+  </si>
+  <si>
+    <t>Star anise</t>
+  </si>
+  <si>
+    <t>Bay leaf</t>
+  </si>
+  <si>
+    <t>Coriander</t>
+  </si>
+  <si>
+    <t>Cinnamon bark</t>
+  </si>
+  <si>
+    <t>Turmeric</t>
+  </si>
+  <si>
+    <t>Curry powder</t>
+  </si>
+  <si>
+    <t>Pepper</t>
+  </si>
+  <si>
+    <t>Nutmeg</t>
+  </si>
+  <si>
+    <t>Cardamom</t>
+  </si>
+  <si>
+    <t>Fennel</t>
+  </si>
+  <si>
+    <t>Chilli flakes</t>
+  </si>
+  <si>
+    <t>Chilli pepper</t>
+  </si>
+  <si>
+    <t>Ginger</t>
+  </si>
+  <si>
+    <t>Cloves</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Vinegar</t>
+  </si>
+  <si>
+    <t>Olive oil</t>
+  </si>
+  <si>
+    <t>Mustard</t>
+  </si>
+  <si>
+    <t>Soy sauce</t>
   </si>
 </sst>
 </file>
@@ -591,15 +726,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AD30F3-BC96-AA4E-AB81-F5562BDF30AC}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -758,44 +895,44 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -803,41 +940,41 @@
         <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -845,55 +982,55 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -901,83 +1038,83 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -985,27 +1122,363 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
         <v>61</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>62</v>
       </c>
-      <c r="D29" t="s">
-        <v>67</v>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+      <c r="D35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" t="s">
+        <v>83</v>
+      </c>
+      <c r="C43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" t="s">
+        <v>112</v>
+      </c>
+      <c r="D53" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added challenge mode for Artikel section.
</commit_message>
<xml_diff>
--- a/data/artikel.xlsx
+++ b/data/artikel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwt/Documents/Code/gelato/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E1343C-B129-864D-82A4-AADD5C7CD206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB99EDF3-FBDD-E042-9E05-E0DC6DC6C3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2D6BCF81-A2D9-5B4D-AD53-B365A8194329}"/>
   </bookViews>
@@ -728,8 +728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AD30F3-BC96-AA4E-AB81-F5562BDF30AC}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added clarity for Ketchup and Salsa.
</commit_message>
<xml_diff>
--- a/data/artikel.xlsx
+++ b/data/artikel.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jwt/Documents/Code/gelato/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E77AF28-8A23-024E-B64C-0759E9B99149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D534919-B7D9-774A-9C3F-9CBB5F6355B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3080" yWindow="2960" windowWidth="21820" windowHeight="14180" xr2:uid="{2D6BCF81-A2D9-5B4D-AD53-B365A8194329}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="174">
   <si>
     <t>Artikel</t>
   </si>
@@ -555,6 +555,9 @@
   </si>
   <si>
     <t>Getränk</t>
+  </si>
+  <si>
+    <t>Salsa (Soßen)</t>
   </si>
 </sst>
 </file>
@@ -906,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AD30F3-BC96-AA4E-AB81-F5562BDF30AC}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="177" zoomScaleNormal="177" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1526,7 +1529,7 @@
         <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>173</v>
       </c>
       <c r="C44" t="s">
         <v>80</v>
@@ -1554,10 +1557,10 @@
         <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="D46" t="s">
         <v>76</v>
@@ -1565,13 +1568,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="D47" t="s">
         <v>76</v>
@@ -1582,10 +1585,10 @@
         <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D48" t="s">
         <v>76</v>
@@ -1596,24 +1599,24 @@
         <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C49" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
       <c r="D49" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D50" t="s">
         <v>117</v>
@@ -1624,10 +1627,10 @@
         <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="C51" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
         <v>117</v>
@@ -1635,13 +1638,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D52" t="s">
         <v>117</v>
@@ -1649,13 +1652,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D53" t="s">
         <v>117</v>
@@ -1663,13 +1666,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D54" t="s">
         <v>117</v>
@@ -1677,13 +1680,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D55" t="s">
         <v>117</v>
@@ -1694,10 +1697,10 @@
         <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D56" t="s">
         <v>117</v>
@@ -1708,10 +1711,10 @@
         <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C57" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D57" t="s">
         <v>117</v>
@@ -1722,10 +1725,10 @@
         <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C58" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D58" t="s">
         <v>117</v>
@@ -1736,10 +1739,10 @@
         <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D59" t="s">
         <v>117</v>
@@ -1750,10 +1753,10 @@
         <v>22</v>
       </c>
       <c r="B60" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D60" t="s">
         <v>117</v>
@@ -1764,10 +1767,10 @@
         <v>22</v>
       </c>
       <c r="B61" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C61" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D61" t="s">
         <v>117</v>
@@ -1775,13 +1778,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B62" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C62" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D62" t="s">
         <v>117</v>
@@ -1789,13 +1792,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C63" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D63" t="s">
         <v>117</v>
@@ -1806,10 +1809,10 @@
         <v>22</v>
       </c>
       <c r="B64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C64" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D64" t="s">
         <v>117</v>
@@ -1817,13 +1820,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D65" t="s">
         <v>117</v>
@@ -1831,13 +1834,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D66" t="s">
         <v>117</v>
@@ -1845,13 +1848,13 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C67" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D67" t="s">
         <v>117</v>
@@ -1859,27 +1862,27 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="C68" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
-        <v>166</v>
+        <v>117</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B69" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C69" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D69" t="s">
         <v>166</v>
@@ -1890,10 +1893,10 @@
         <v>25</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C70" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D70" t="s">
         <v>166</v>
@@ -1901,13 +1904,13 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C71" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D71" t="s">
         <v>166</v>
@@ -1915,13 +1918,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B72" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D72" t="s">
         <v>166</v>
@@ -1929,13 +1932,13 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C73" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D73" t="s">
         <v>166</v>
@@ -1946,10 +1949,10 @@
         <v>22</v>
       </c>
       <c r="B74" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
       <c r="C74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D74" t="s">
         <v>166</v>
@@ -1960,10 +1963,10 @@
         <v>22</v>
       </c>
       <c r="B75" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C75" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D75" t="s">
         <v>166</v>
@@ -1971,13 +1974,13 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B76" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D76" t="s">
         <v>166</v>
@@ -1988,10 +1991,10 @@
         <v>25</v>
       </c>
       <c r="B77" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C77" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D77" t="s">
         <v>166</v>
@@ -2002,10 +2005,10 @@
         <v>25</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D78" t="s">
         <v>166</v>
@@ -2016,10 +2019,10 @@
         <v>25</v>
       </c>
       <c r="B79" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C79" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D79" t="s">
         <v>166</v>
@@ -2030,10 +2033,10 @@
         <v>25</v>
       </c>
       <c r="B80" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C80" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D80" t="s">
         <v>166</v>
@@ -2041,13 +2044,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="C81" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D81" t="s">
         <v>166</v>
@@ -2055,15 +2058,29 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B82" t="s">
+        <v>162</v>
+      </c>
+      <c r="C82" t="s">
+        <v>163</v>
+      </c>
+      <c r="D82" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>25</v>
+      </c>
+      <c r="B83" t="s">
         <v>164</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C83" t="s">
         <v>165</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D83" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>